<commit_message>
finished the fixes, added markup and free ongkir
</commit_message>
<xml_diff>
--- a/update_shopee/SETTINGS/constant.xlsx
+++ b/update_shopee/SETTINGS/constant.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edenmac/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edenmac/Programs/maxi-onlineshop/update_shopee/SETTINGS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A307A898-D158-524C-AF3D-72C292F743A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E505B728-3244-1945-9725-4A227B7DBEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="16820" xr2:uid="{81F1896D-4173-4A4D-B1A3-4673B31B25B4}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>STOCK_DIVISOR</t>
   </si>
   <si>
     <t>FREE_ONGKIR_FEE</t>
+  </si>
+  <si>
+    <t>MARKUP</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAA803F-A50C-AA42-B35B-162AF628E9D1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,6 +443,14 @@
         <v>0.04</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>